<commit_message>
acrescentei "meat" e "check grill" às opções para schedule event e corrigi nos dados "cleanig" (faltava o "n")
</commit_message>
<xml_diff>
--- a/datasetKDB.xlsx
+++ b/datasetKDB.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="39">
   <si>
     <t>source</t>
   </si>
@@ -135,13 +135,10 @@
     <t>Barbecue</t>
   </si>
   <si>
-    <t>cleanig Service</t>
-  </si>
-  <si>
     <t>new3</t>
   </si>
   <si>
-    <t>cleanig service</t>
+    <t>cleaning Service</t>
   </si>
 </sst>
 </file>
@@ -648,7 +645,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="437">
+  <cellXfs count="457">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="42">
       <alignment wrapText="1"/>
@@ -672,6 +669,66 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="42">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="43">
@@ -2284,10 +2341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,25 +2382,25 @@
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="117" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="171" t="s">
+      <c r="B2" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="121" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="177" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="224" t="s">
+      <c r="E2" s="232" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="278" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="328" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="382" t="s">
+      <c r="F2" s="288" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="344" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="400" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2351,25 +2408,25 @@
       <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="118" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="172" t="s">
+      <c r="B3" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="122" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="178" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="225" t="s">
+      <c r="E3" s="233" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="279" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="329" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="383" t="s">
+      <c r="F3" s="289" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="345" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="401" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2377,25 +2434,25 @@
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="119" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="173" t="s">
+      <c r="B4" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="123" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="179" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="226" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="280" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="330" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="384" t="s">
+      <c r="E4" s="234" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="290" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="346" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="402" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2403,25 +2460,25 @@
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="120" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="174" t="s">
+      <c r="B5" s="68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="124" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="227" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="281" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="331" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="385" t="s">
+      <c r="E5" s="235" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="291" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="347" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="403" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2429,25 +2486,25 @@
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="121" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="175" t="s">
+      <c r="B6" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="125" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="181" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="228" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="282" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="332" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="386" t="s">
+      <c r="E6" s="236" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="292" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="348" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="404" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2455,25 +2512,25 @@
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="122" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="176" t="s">
+      <c r="B7" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="126" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="182" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="229" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="283" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="333" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="387" t="s">
+      <c r="E7" s="237" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="293" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="349" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="405" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2481,25 +2538,25 @@
       <c r="A8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="123" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="177" t="s">
+      <c r="B8" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="127" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="183" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="230" t="s">
+      <c r="E8" s="238" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="284" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="334" t="s">
+      <c r="F8" s="294" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="350" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="388" t="s">
+      <c r="H8" s="406" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2507,25 +2564,25 @@
       <c r="A9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="124" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="178" t="s">
+      <c r="B9" s="72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="128" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="184" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="231" t="s">
+      <c r="E9" s="239" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="285" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="335" t="s">
+      <c r="F9" s="295" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="351" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="389" t="s">
+      <c r="H9" s="407" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2533,25 +2590,25 @@
       <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="125" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="179" t="s">
+      <c r="B10" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="185" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="232" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="286" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="336" t="s">
+      <c r="E10" s="240" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="296" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="352" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="390" t="s">
+      <c r="H10" s="408" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2559,25 +2616,25 @@
       <c r="A11" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="126" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="180" t="s">
+      <c r="B11" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="130" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="186" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="233" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="287" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="337" t="s">
+      <c r="E11" s="241" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="297" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="353" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="391" t="s">
+      <c r="H11" s="409" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2585,25 +2642,25 @@
       <c r="A12" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="127" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="181" t="s">
+      <c r="B12" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="131" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="187" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="234" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="288" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="338" t="s">
+      <c r="E12" s="242" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="298" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="354" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="392" t="s">
+      <c r="H12" s="410" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2611,25 +2668,25 @@
       <c r="A13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="128" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="182" t="s">
+      <c r="B13" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="132" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="188" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="235" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" s="289" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13" s="339" t="s">
+      <c r="E13" s="243" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="299" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="355" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="393" t="s">
+      <c r="H13" s="411" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2637,25 +2694,25 @@
       <c r="A14" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="129" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="183" t="s">
+      <c r="B14" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="133" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="189" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="236" t="s">
+      <c r="E14" s="244" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="290" t="s">
+      <c r="F14" s="300" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="340" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="394" t="s">
+      <c r="G14" s="356" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="412" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2663,25 +2720,25 @@
       <c r="A15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="130" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="184" t="s">
+      <c r="B15" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="134" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="190" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="237" t="s">
+      <c r="E15" s="245" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="291" t="s">
+      <c r="F15" s="301" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="341" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="395" t="s">
+      <c r="G15" s="357" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="413" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2689,25 +2746,25 @@
       <c r="A16" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="77" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="131" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="185" t="s">
+      <c r="B16" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="135" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="191" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="238" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="292" t="s">
+      <c r="E16" s="246" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="302" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="342" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="396" t="s">
+      <c r="G16" s="358" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="414" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2715,25 +2772,25 @@
       <c r="A17" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="78" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="132" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="186" t="s">
+      <c r="B17" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="136" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="239" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="293" t="s">
+      <c r="E17" s="247" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="303" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="343" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="397" t="s">
+      <c r="G17" s="359" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="415" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2741,25 +2798,25 @@
       <c r="A18" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="133" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="187" t="s">
+      <c r="B18" s="81" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="137" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="240" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="294" t="s">
+      <c r="E18" s="248" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="304" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="344" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="398" t="s">
+      <c r="G18" s="360" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="416" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2767,25 +2824,25 @@
       <c r="A19" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="134" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="188" t="s">
+      <c r="B19" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="138" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="194" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="241" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="295" t="s">
+      <c r="E19" s="249" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="305" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="345" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="399" t="s">
+      <c r="G19" s="361" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="417" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2793,25 +2850,25 @@
       <c r="A20" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="135" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="189" t="s">
+      <c r="B20" s="83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="139" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="195" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="242" t="s">
+      <c r="E20" s="250" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="296" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="346" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="400" t="s">
+      <c r="F20" s="306" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="362" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="418" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2819,25 +2876,25 @@
       <c r="A21" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="82" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="136" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="190" t="s">
+      <c r="B21" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="140" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="196" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="243" t="s">
+      <c r="E21" s="251" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="297" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="347" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="401" t="s">
+      <c r="F21" s="307" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="363" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="419" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2845,25 +2902,25 @@
       <c r="A22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="83" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="137" t="s">
-        <v>36</v>
-      </c>
-      <c r="D22" s="191" t="s">
+      <c r="B22" s="85" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="141" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="197" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="244" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" s="298" t="s">
-        <v>18</v>
-      </c>
-      <c r="G22" s="348" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="402" t="s">
+      <c r="E22" s="252" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="308" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="364" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="420" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2871,25 +2928,25 @@
       <c r="A23" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="138" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="192" t="s">
+      <c r="B23" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="142" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="198" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="245" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="299" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="349" t="s">
-        <v>16</v>
-      </c>
-      <c r="H23" s="403" t="s">
+      <c r="E23" s="253" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="309" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="365" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="421" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2897,25 +2954,25 @@
       <c r="A24" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="85" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="139" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="193" t="s">
+      <c r="B24" s="87" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="143" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="199" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="246" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="300" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24" s="350" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="404" t="s">
+      <c r="E24" s="254" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="310" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="366" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="422" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2923,25 +2980,25 @@
       <c r="A25" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="86" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="140" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="194" t="s">
+      <c r="B25" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="144" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="200" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="247" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" s="301" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="351" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="405" t="s">
+      <c r="E25" s="255" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="311" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="367" t="s">
+        <v>16</v>
+      </c>
+      <c r="H25" s="423" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2949,25 +3006,25 @@
       <c r="A26" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="87" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" s="141" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="195" t="s">
+      <c r="B26" s="89" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="145" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="201" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="248" t="s">
+      <c r="E26" s="256" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="302" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="352" t="s">
-        <v>16</v>
-      </c>
-      <c r="H26" s="406" t="s">
+      <c r="F26" s="312" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="368" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="424" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2975,25 +3032,25 @@
       <c r="A27" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="88" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="142" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="196" t="s">
+      <c r="B27" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="146" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="249" t="s">
+      <c r="E27" s="257" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="303" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="353" t="s">
-        <v>16</v>
-      </c>
-      <c r="H27" s="407" t="s">
+      <c r="F27" s="313" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="369" t="s">
+        <v>16</v>
+      </c>
+      <c r="H27" s="425" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3001,25 +3058,25 @@
       <c r="A28" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="89" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="143" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="197" t="s">
+      <c r="B28" s="91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="203" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="250" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="304" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="354" t="s">
-        <v>16</v>
-      </c>
-      <c r="H28" s="408" t="s">
+      <c r="E28" s="258" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="314" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="370" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="426" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3027,25 +3084,25 @@
       <c r="A29" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="90" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="144" t="s">
-        <v>36</v>
-      </c>
-      <c r="D29" s="198" t="s">
+      <c r="B29" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="148" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="204" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="251" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" s="305" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29" s="355" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="409" t="s">
+      <c r="E29" s="259" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="315" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="371" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="427" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3053,25 +3110,25 @@
       <c r="A30" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="91" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="145" t="s">
-        <v>36</v>
-      </c>
-      <c r="D30" s="199" t="s">
+      <c r="B30" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="252" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="306" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="356" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="410" t="s">
+      <c r="E30" s="260" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="316" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30" s="372" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="428" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3079,25 +3136,25 @@
       <c r="A31" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="92" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="146" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="200" t="s">
+      <c r="B31" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="150" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="206" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="253" t="s">
+      <c r="E31" s="261" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="307" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="357" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="411" t="s">
+      <c r="F31" s="317" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="373" t="s">
+        <v>16</v>
+      </c>
+      <c r="H31" s="429" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3105,25 +3162,25 @@
       <c r="A32" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="147" t="s">
-        <v>36</v>
-      </c>
-      <c r="D32" s="201" t="s">
+      <c r="B32" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="151" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="207" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="254" t="s">
+      <c r="E32" s="262" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="308" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="358" t="s">
-        <v>16</v>
-      </c>
-      <c r="H32" s="412" t="s">
+      <c r="F32" s="318" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="374" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="430" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3131,25 +3188,25 @@
       <c r="A33" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="148" t="s">
-        <v>36</v>
-      </c>
-      <c r="D33" s="202" t="s">
+      <c r="B33" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="152" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="255" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="309" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="359" t="s">
-        <v>16</v>
-      </c>
-      <c r="H33" s="413" t="s">
+      <c r="E33" s="263" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="319" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="375" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="431" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3157,25 +3214,25 @@
       <c r="A34" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="95" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="203" t="s">
+      <c r="B34" s="97" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="153" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="209" t="s">
         <v>32</v>
       </c>
-      <c r="E34" s="256" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" s="310" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="360" t="s">
-        <v>16</v>
-      </c>
-      <c r="H34" s="414" t="s">
+      <c r="E34" s="264" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="320" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="376" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="432" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3183,25 +3240,25 @@
       <c r="A35" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="96" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="150" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="204" t="s">
+      <c r="B35" s="98" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="154" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="210" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="257" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" s="311" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="361" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="415" t="s">
+      <c r="E35" s="265" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="321" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" s="377" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="433" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3209,520 +3266,572 @@
       <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="97" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="151" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="205" t="s">
+      <c r="B36" s="99" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="155" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="211" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="266" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" s="322" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="378" t="s">
+        <v>16</v>
+      </c>
+      <c r="H36" s="434" t="s">
         <v>37</v>
-      </c>
-      <c r="E36" s="258" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36" s="312" t="s">
-        <v>18</v>
-      </c>
-      <c r="G36" s="362" t="s">
-        <v>16</v>
-      </c>
-      <c r="H36" s="416" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="98" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="152" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="206" t="s">
+      <c r="B37" s="100" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="156" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="212" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="267" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" s="323" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="379" t="s">
+        <v>16</v>
+      </c>
+      <c r="H37" s="435" t="s">
         <v>37</v>
-      </c>
-      <c r="E37" s="259" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" s="313" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="363" t="s">
-        <v>16</v>
-      </c>
-      <c r="H37" s="417" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="99" t="s">
-        <v>33</v>
-      </c>
-      <c r="C38" s="153" t="s">
-        <v>36</v>
-      </c>
-      <c r="D38" s="207" t="s">
+      <c r="B38" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="157" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="213" t="s">
         <v>27</v>
       </c>
-      <c r="E38" s="260" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="314" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="364" t="s">
-        <v>16</v>
-      </c>
-      <c r="H38" s="418" t="s">
-        <v>38</v>
+      <c r="E38" s="268" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="324" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="380" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="436" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="100" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="154" t="s">
-        <v>36</v>
-      </c>
-      <c r="D39" s="208" t="s">
+      <c r="B39" s="102" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="158" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" s="214" t="s">
         <v>27</v>
       </c>
-      <c r="E39" s="261" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="315" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="365" t="s">
-        <v>16</v>
-      </c>
-      <c r="H39" s="419" t="s">
-        <v>38</v>
+      <c r="E39" s="269" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="325" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="381" t="s">
+        <v>16</v>
+      </c>
+      <c r="H39" s="437" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="101" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="155" t="s">
-        <v>36</v>
-      </c>
-      <c r="D40" s="209" t="s">
+      <c r="B40" s="103" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="159" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="215" t="s">
         <v>28</v>
       </c>
-      <c r="E40" s="262" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" s="316" t="s">
-        <v>18</v>
-      </c>
-      <c r="G40" s="366" t="s">
-        <v>16</v>
-      </c>
-      <c r="H40" s="420" t="s">
-        <v>38</v>
+      <c r="E40" s="270" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="326" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="382" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="438" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="156" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="210" t="s">
+      <c r="B41" s="104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="160" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" s="216" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="263" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" s="317" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="367" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="421" t="s">
-        <v>38</v>
+      <c r="E41" s="271" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="327" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="383" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="439" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="103" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="157" t="s">
-        <v>36</v>
-      </c>
-      <c r="D42" s="211" t="s">
+      <c r="B42" s="105" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="161" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="264" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" s="318" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="368" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="422" t="s">
-        <v>38</v>
+      <c r="E42" s="272" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="328" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="384" t="s">
+        <v>16</v>
+      </c>
+      <c r="H42" s="440" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="104" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="158" t="s">
-        <v>36</v>
-      </c>
-      <c r="D43" s="212" t="s">
+      <c r="B43" s="106" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="162" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="265" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" s="319" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="369" t="s">
-        <v>16</v>
-      </c>
-      <c r="H43" s="423" t="s">
-        <v>38</v>
+      <c r="E43" s="273" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="329" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="385" t="s">
+        <v>16</v>
+      </c>
+      <c r="H43" s="441" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B44" s="105" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="159" t="s">
-        <v>36</v>
-      </c>
-      <c r="D44" s="213" t="s">
+      <c r="B44" s="107" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="163" t="s">
+        <v>36</v>
+      </c>
+      <c r="D44" s="219" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="266" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" s="320" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="370" t="s">
-        <v>16</v>
-      </c>
-      <c r="H44" s="424" t="s">
-        <v>38</v>
+      <c r="E44" s="274" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="330" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="386" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="442" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="106" t="s">
-        <v>33</v>
-      </c>
-      <c r="C45" s="160" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="214" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="267" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="321" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="371" t="s">
-        <v>16</v>
-      </c>
-      <c r="H45" s="425" t="s">
-        <v>38</v>
+      <c r="B45" s="108" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="164" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="220" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="275" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="331" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="387" t="s">
+        <v>16</v>
+      </c>
+      <c r="H45" s="443" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="107" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="161" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="215" t="s">
+      <c r="B46" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="165" t="s">
+        <v>36</v>
+      </c>
+      <c r="D46" s="221" t="s">
         <v>27</v>
       </c>
-      <c r="E46" s="268" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" s="322" t="s">
-        <v>18</v>
-      </c>
-      <c r="G46" s="372" t="s">
-        <v>16</v>
-      </c>
-      <c r="H46" s="426" t="s">
-        <v>38</v>
+      <c r="E46" s="276" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="332" t="s">
+        <v>18</v>
+      </c>
+      <c r="G46" s="388" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="444" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="162" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="216" t="s">
+      <c r="B47" s="110" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" s="166" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="269" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="323" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="373" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="427" t="s">
-        <v>38</v>
+      <c r="E47" s="277" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="333" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="389" t="s">
+        <v>16</v>
+      </c>
+      <c r="H47" s="445" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B48" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="C48" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="217" t="s">
+      <c r="B48" s="111" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="167" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="223" t="s">
         <v>28</v>
       </c>
-      <c r="E48" s="270" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" s="324" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="374" t="s">
-        <v>16</v>
-      </c>
-      <c r="H48" s="428" t="s">
-        <v>38</v>
+      <c r="E48" s="278" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="334" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="390" t="s">
+        <v>16</v>
+      </c>
+      <c r="H48" s="446" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="C49" s="164" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="218" t="s">
+      <c r="B49" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="168" t="s">
+        <v>36</v>
+      </c>
+      <c r="D49" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="E49" s="271" t="s">
-        <v>12</v>
-      </c>
-      <c r="F49" s="325" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="375" t="s">
-        <v>16</v>
-      </c>
-      <c r="H49" s="429" t="s">
-        <v>38</v>
+      <c r="E49" s="279" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="335" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="391" t="s">
+        <v>16</v>
+      </c>
+      <c r="H49" s="447" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="111" t="s">
-        <v>33</v>
-      </c>
-      <c r="C50" s="165" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="219" t="s">
+      <c r="B50" s="113" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="169" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="225" t="s">
         <v>27</v>
       </c>
-      <c r="E50" s="272" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" s="326" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="376" t="s">
-        <v>16</v>
-      </c>
-      <c r="H50" s="430" t="s">
-        <v>38</v>
+      <c r="E50" s="280" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="336" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="392" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="448" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="112" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="166" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="220" t="s">
+      <c r="B51" s="114" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="170" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="226" t="s">
         <v>27</v>
       </c>
-      <c r="E51" s="273" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" s="435" t="s">
+      <c r="E51" s="281" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="337" t="s">
         <v>19</v>
       </c>
-      <c r="G51" s="377" t="s">
-        <v>16</v>
-      </c>
-      <c r="H51" s="431" t="s">
-        <v>38</v>
+      <c r="G51" s="393" t="s">
+        <v>16</v>
+      </c>
+      <c r="H51" s="449" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B52" s="113" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="167" t="s">
-        <v>36</v>
-      </c>
-      <c r="D52" s="436" t="s">
+      <c r="B52" s="115" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="171" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="227" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="274" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" s="435" t="s">
+      <c r="E52" s="282" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="338" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="378" t="s">
-        <v>16</v>
-      </c>
-      <c r="H52" s="432" t="s">
-        <v>38</v>
+      <c r="G52" s="394" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="450" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="114" t="s">
-        <v>33</v>
-      </c>
-      <c r="C53" s="168" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="221" t="s">
+      <c r="B53" s="116" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="228" t="s">
         <v>27</v>
       </c>
-      <c r="E53" s="275" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="435" t="s">
+      <c r="E53" s="283" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="339" t="s">
         <v>19</v>
       </c>
-      <c r="G53" s="379" t="s">
-        <v>16</v>
-      </c>
-      <c r="H53" s="433" t="s">
-        <v>38</v>
+      <c r="G53" s="395" t="s">
+        <v>16</v>
+      </c>
+      <c r="H53" s="451" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B54" s="115" t="s">
-        <v>33</v>
-      </c>
-      <c r="C54" s="169" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="222" t="s">
+      <c r="B54" s="117" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="173" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="229" t="s">
         <v>27</v>
       </c>
-      <c r="E54" s="276" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" s="435" t="s">
+      <c r="E54" s="284" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="340" t="s">
         <v>19</v>
       </c>
-      <c r="G54" s="380" t="s">
-        <v>16</v>
-      </c>
-      <c r="H54" s="434" t="s">
-        <v>38</v>
+      <c r="G54" s="396" t="s">
+        <v>16</v>
+      </c>
+      <c r="H54" s="452" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="116" t="s">
-        <v>33</v>
-      </c>
-      <c r="C55" s="170" t="s">
-        <v>36</v>
-      </c>
-      <c r="D55" s="223" t="s">
+      <c r="B55" s="118" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="174" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="230" t="s">
         <v>27</v>
       </c>
-      <c r="E55" s="277" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" s="327" t="s">
+      <c r="E55" s="285" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="341" t="s">
         <v>19</v>
       </c>
-      <c r="G55" s="381" t="s">
-        <v>16</v>
-      </c>
-      <c r="H55" s="435" t="s">
-        <v>38</v>
+      <c r="G55" s="397" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="453" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="175" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" s="231" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="286" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="342" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="398" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="454" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="120" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="176" t="s">
+        <v>36</v>
+      </c>
+      <c r="D57" s="456" t="s">
+        <v>32</v>
+      </c>
+      <c r="E57" s="287" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" s="343" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="399" t="s">
+        <v>16</v>
+      </c>
+      <c r="H57" s="455" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>